<commit_message>
Due to slow problem in openpyxl, switch to pandas and it is so fast
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,17 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="480" yWindow="105" windowWidth="27795" windowHeight="12600"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -234,38 +232,38 @@
     <t>03-JUN-29 12.00.00.000000000 AM</t>
   </si>
   <si>
-    <t>ID</t>
+    <t>issue_date</t>
+  </si>
+  <si>
+    <t>DL</t>
   </si>
   <si>
     <t>Ref</t>
   </si>
   <si>
-    <t>DL</t>
-  </si>
-  <si>
-    <t>App_Status</t>
-  </si>
-  <si>
-    <t>Card_Status</t>
-  </si>
-  <si>
-    <t>Afis_Status</t>
-  </si>
-  <si>
-    <t>Issue_Date</t>
-  </si>
-  <si>
-    <t>Expiry_Date</t>
-  </si>
-  <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Expiry_date</t>
+  </si>
+  <si>
+    <t>afis_Status</t>
+  </si>
+  <si>
+    <t>card_Status</t>
+  </si>
+  <si>
+    <t>App_status</t>
+  </si>
+  <si>
+    <t>iD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -273,16 +271,317 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -290,18 +589,209 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -597,50 +1087,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I20"/>
+  <dimension ref="A1:I131533"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="28.7109375" customWidth="1"/>
-    <col min="3" max="3" width="25.7109375" customWidth="1"/>
-    <col min="4" max="4" width="15.140625" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="17.5703125" customWidth="1"/>
-    <col min="7" max="7" width="60.28515625" customWidth="1"/>
-    <col min="8" max="8" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="8" max="8" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>73</v>
       </c>
-      <c r="C1" t="s">
-        <v>74</v>
-      </c>
       <c r="D1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="E1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F1" t="s">
         <v>77</v>
       </c>
       <c r="G1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="H1" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I1" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -656,9 +1141,6 @@
       <c r="D2">
         <v>53</v>
       </c>
-      <c r="E2">
-        <v>187</v>
-      </c>
       <c r="F2">
         <v>95</v>
       </c>
@@ -1194,31 +1676,19 @@
         <v>1</v>
       </c>
     </row>
+    <row r="43512" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B43512" s="1"/>
+    </row>
+    <row r="95620" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95620" s="2"/>
+    </row>
+    <row r="130751" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130751" s="1"/>
+    </row>
+    <row r="131533" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131533" s="1"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>